<commit_message>
resolve stash merge conflicts
</commit_message>
<xml_diff>
--- a/my_scripts/transect_SZ.xlsx
+++ b/my_scripts/transect_SZ.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cygwin64\home\Takashi\COAWST\matlab\my_scripts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\takahashi\COAWST\matlab\my_scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BB5CF43-50CD-467A-AD8D-0E90FC0A2E52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2D02D63-FAAB-4E50-886C-4E2A167ADDFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16680" yWindow="780" windowWidth="15168" windowHeight="11952" xr2:uid="{68DBF74F-1B36-4EFF-8658-3C9C1DBE3C27}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{68DBF74F-1B36-4EFF-8658-3C9C1DBE3C27}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
   <si>
     <t>transect1</t>
     <phoneticPr fontId="1"/>
@@ -40,6 +40,10 @@
   </si>
   <si>
     <t>transect2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>transect3</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -101,7 +105,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -117,9 +121,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 テーマ">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -157,7 +161,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -263,7 +267,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -405,7 +409,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -413,23 +417,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DBB84A2-4B23-417B-8F55-173E4F56F21E}">
-  <dimension ref="A1:D141"/>
+  <dimension ref="A1:F141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A107" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F104" sqref="F104"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -442,8 +449,14 @@
       <c r="D2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>16</v>
       </c>
@@ -456,8 +469,14 @@
       <c r="D3">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E3">
+        <v>23</v>
+      </c>
+      <c r="F3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>17</v>
       </c>
@@ -471,7 +490,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>18</v>
       </c>
@@ -485,7 +504,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>19</v>
       </c>
@@ -499,7 +518,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>20</v>
       </c>
@@ -513,7 +532,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>21</v>
       </c>
@@ -527,7 +546,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>22</v>
       </c>
@@ -541,7 +560,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>23</v>
       </c>
@@ -555,7 +574,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>24</v>
       </c>
@@ -569,7 +588,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>25</v>
       </c>
@@ -583,7 +602,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A13">
         <v>26</v>
       </c>
@@ -597,7 +616,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A14">
         <v>27</v>
       </c>
@@ -611,7 +630,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A15">
         <v>28</v>
       </c>
@@ -625,7 +644,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A16">
         <v>29</v>
       </c>
@@ -639,7 +658,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A17">
         <v>30</v>
       </c>
@@ -653,7 +672,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A18">
         <v>31</v>
       </c>
@@ -667,7 +686,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A19">
         <v>32</v>
       </c>
@@ -681,7 +700,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A20">
         <v>33</v>
       </c>
@@ -695,7 +714,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A21">
         <v>34</v>
       </c>
@@ -709,7 +728,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A22">
         <v>35</v>
       </c>
@@ -723,7 +742,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A23">
         <v>36</v>
       </c>
@@ -737,7 +756,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A24">
         <v>37</v>
       </c>
@@ -751,7 +770,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A25">
         <v>38</v>
       </c>
@@ -765,7 +784,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A26">
         <v>39</v>
       </c>
@@ -779,7 +798,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A27">
         <v>40</v>
       </c>
@@ -793,7 +812,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A28">
         <v>41</v>
       </c>
@@ -807,7 +826,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A29">
         <v>42</v>
       </c>
@@ -821,7 +840,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A30">
         <v>43</v>
       </c>
@@ -835,7 +854,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A31">
         <v>44</v>
       </c>
@@ -849,7 +868,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A32">
         <v>45</v>
       </c>
@@ -863,7 +882,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A33">
         <v>46</v>
       </c>
@@ -877,7 +896,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A34">
         <v>47</v>
       </c>
@@ -891,7 +910,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A35">
         <v>48</v>
       </c>
@@ -905,7 +924,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A36">
         <v>49</v>
       </c>
@@ -919,7 +938,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A37">
         <v>50</v>
       </c>
@@ -933,7 +952,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A38">
         <v>51</v>
       </c>
@@ -947,7 +966,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A39">
         <v>52</v>
       </c>
@@ -961,7 +980,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A40">
         <v>53</v>
       </c>
@@ -975,7 +994,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A41">
         <v>54</v>
       </c>
@@ -989,7 +1008,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A42">
         <v>55</v>
       </c>
@@ -1003,7 +1022,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A43">
         <v>56</v>
       </c>
@@ -1017,7 +1036,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A44">
         <v>57</v>
       </c>
@@ -1031,7 +1050,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A45">
         <v>58</v>
       </c>
@@ -1045,7 +1064,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A46">
         <v>59</v>
       </c>
@@ -1059,7 +1078,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A47">
         <v>60</v>
       </c>
@@ -1073,7 +1092,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A48">
         <v>61</v>
       </c>
@@ -1087,7 +1106,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A49">
         <v>62</v>
       </c>
@@ -1101,7 +1120,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A50">
         <v>63</v>
       </c>
@@ -1115,7 +1134,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A51">
         <v>64</v>
       </c>
@@ -1129,7 +1148,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A52">
         <v>65</v>
       </c>
@@ -1143,7 +1162,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A53">
         <v>66</v>
       </c>
@@ -1157,7 +1176,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A54">
         <v>67</v>
       </c>
@@ -1171,7 +1190,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A55">
         <v>68</v>
       </c>
@@ -1185,7 +1204,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A56">
         <v>69</v>
       </c>
@@ -1199,7 +1218,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A57">
         <v>70</v>
       </c>
@@ -1213,7 +1232,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A58">
         <v>71</v>
       </c>
@@ -1227,7 +1246,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A59">
         <v>72</v>
       </c>
@@ -1241,7 +1260,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A60">
         <v>73</v>
       </c>
@@ -1255,7 +1274,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A61">
         <v>74</v>
       </c>
@@ -1269,7 +1288,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A62">
         <v>75</v>
       </c>
@@ -1283,7 +1302,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A63">
         <v>76</v>
       </c>
@@ -1297,7 +1316,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A64">
         <v>77</v>
       </c>
@@ -1311,7 +1330,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A65">
         <v>78</v>
       </c>
@@ -1325,7 +1344,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A66">
         <v>79</v>
       </c>
@@ -1339,7 +1358,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A67">
         <v>80</v>
       </c>
@@ -1353,7 +1372,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A68">
         <v>81</v>
       </c>
@@ -1367,7 +1386,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A69">
         <v>82</v>
       </c>
@@ -1381,7 +1400,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A70">
         <v>83</v>
       </c>
@@ -1395,7 +1414,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A71">
         <v>84</v>
       </c>
@@ -1409,7 +1428,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A72">
         <v>85</v>
       </c>
@@ -1423,7 +1442,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A73">
         <v>86</v>
       </c>
@@ -1437,7 +1456,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A74">
         <v>87</v>
       </c>
@@ -1451,7 +1470,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A75">
         <v>88</v>
       </c>
@@ -1465,7 +1484,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A76">
         <v>89</v>
       </c>
@@ -1479,7 +1498,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A77">
         <v>90</v>
       </c>
@@ -1493,7 +1512,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A78">
         <v>90</v>
       </c>
@@ -1507,7 +1526,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A79">
         <v>91</v>
       </c>
@@ -1521,7 +1540,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A80">
         <v>92</v>
       </c>
@@ -1535,7 +1554,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A81">
         <v>92</v>
       </c>
@@ -1549,7 +1568,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A82">
         <v>93</v>
       </c>
@@ -1563,7 +1582,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A83">
         <v>94</v>
       </c>
@@ -1577,7 +1596,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A84">
         <v>94</v>
       </c>
@@ -1591,7 +1610,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A85">
         <v>95</v>
       </c>
@@ -1605,7 +1624,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A86">
         <v>96</v>
       </c>
@@ -1619,7 +1638,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A87">
         <v>96</v>
       </c>
@@ -1633,7 +1652,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A88">
         <v>97</v>
       </c>
@@ -1647,7 +1666,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A89">
         <v>98</v>
       </c>
@@ -1661,7 +1680,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A90">
         <v>98</v>
       </c>
@@ -1675,7 +1694,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A91">
         <v>99</v>
       </c>
@@ -1689,7 +1708,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A92">
         <v>100</v>
       </c>
@@ -1703,7 +1722,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A93">
         <v>100</v>
       </c>
@@ -1717,7 +1736,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A94">
         <v>101</v>
       </c>
@@ -1731,7 +1750,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A95">
         <v>102</v>
       </c>
@@ -1745,7 +1764,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A96">
         <v>102</v>
       </c>
@@ -1759,7 +1778,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A97">
         <v>103</v>
       </c>
@@ -1773,7 +1792,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A98">
         <v>104</v>
       </c>
@@ -1787,7 +1806,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A99">
         <v>104</v>
       </c>
@@ -1801,7 +1820,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A100">
         <v>105</v>
       </c>
@@ -1815,7 +1834,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A101">
         <v>106</v>
       </c>
@@ -1829,7 +1848,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A102">
         <v>106</v>
       </c>
@@ -1843,7 +1862,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A103">
         <v>107</v>
       </c>
@@ -1857,7 +1876,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A104">
         <v>108</v>
       </c>
@@ -1871,7 +1890,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A105">
         <v>109</v>
       </c>
@@ -1885,7 +1904,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A106">
         <v>110</v>
       </c>
@@ -1899,7 +1918,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A107">
         <v>111</v>
       </c>
@@ -1913,7 +1932,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A108">
         <v>112</v>
       </c>
@@ -1927,7 +1946,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A109">
         <v>113</v>
       </c>
@@ -1941,7 +1960,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A110">
         <v>114</v>
       </c>
@@ -1955,7 +1974,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A111">
         <v>115</v>
       </c>
@@ -1969,7 +1988,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A112">
         <v>116</v>
       </c>
@@ -1983,7 +2002,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A113">
         <v>117</v>
       </c>
@@ -1997,7 +2016,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A114">
         <v>118</v>
       </c>
@@ -2011,7 +2030,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A115">
         <v>119</v>
       </c>
@@ -2025,7 +2044,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A116">
         <v>120</v>
       </c>
@@ -2039,7 +2058,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A117">
         <v>121</v>
       </c>
@@ -2053,7 +2072,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A118">
         <v>122</v>
       </c>
@@ -2067,7 +2086,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A119">
         <v>123</v>
       </c>
@@ -2081,7 +2100,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A120">
         <v>124</v>
       </c>
@@ -2095,7 +2114,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A121">
         <v>125</v>
       </c>
@@ -2109,7 +2128,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A122">
         <v>126</v>
       </c>
@@ -2123,7 +2142,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A123">
         <v>127</v>
       </c>
@@ -2137,7 +2156,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A124">
         <v>128</v>
       </c>
@@ -2151,7 +2170,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A125">
         <v>129</v>
       </c>
@@ -2165,7 +2184,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A126">
         <v>130</v>
       </c>
@@ -2179,7 +2198,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A127">
         <v>131</v>
       </c>
@@ -2193,7 +2212,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A128">
         <v>132</v>
       </c>
@@ -2207,7 +2226,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A129">
         <v>133</v>
       </c>
@@ -2221,7 +2240,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A130">
         <v>134</v>
       </c>
@@ -2235,7 +2254,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A131">
         <v>135</v>
       </c>
@@ -2249,7 +2268,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A132">
         <v>136</v>
       </c>
@@ -2263,7 +2282,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A133">
         <v>137</v>
       </c>
@@ -2277,7 +2296,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A134">
         <v>138</v>
       </c>
@@ -2291,7 +2310,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A135">
         <v>139</v>
       </c>
@@ -2305,7 +2324,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A136">
         <v>140</v>
       </c>
@@ -2319,7 +2338,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A137">
         <v>141</v>
       </c>
@@ -2333,7 +2352,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A138">
         <v>142</v>
       </c>
@@ -2347,7 +2366,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A139">
         <v>143</v>
       </c>
@@ -2355,7 +2374,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A140">
         <v>144</v>
       </c>
@@ -2363,7 +2382,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A141">
         <v>145</v>
       </c>

</xml_diff>